<commit_message>
room type selections added
</commit_message>
<xml_diff>
--- a/HotelPriceCalculator/Data/FUN SUN CLUB SAPHIRE.xlsx
+++ b/HotelPriceCalculator/Data/FUN SUN CLUB SAPHIRE.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odabasi\source\repos\HotelPriceCalculator\HotelPriceCalculator\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6810" tabRatio="889"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34728" windowHeight="17724" tabRatio="889"/>
   </bookViews>
   <sheets>
     <sheet name="FUN SUN CLUB SAPHİRE" sheetId="4" r:id="rId1"/>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'FUN SUN CLUB SAPHİRE'!$A$1:$K$36</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -88,7 +93,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00\ _T_L"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;TL&quot;"/>
@@ -1622,9 +1627,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Ofis Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
-    <a:clrScheme name="Ofis">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1662,9 +1667,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Ofis">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1699,7 +1704,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1734,7 +1739,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Ofis">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1914,14 +1919,14 @@
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="24.375" customWidth="1"/>
+    <col min="1" max="1" width="24.3984375" customWidth="1"/>
     <col min="2" max="2" width="6.5" style="14" customWidth="1"/>
     <col min="3" max="11" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1">
+    <row r="1" spans="1:11" ht="16.2" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="10"/>
       <c r="C1" s="2"/>
@@ -1990,7 +1995,7 @@
       <c r="J5" s="97"/>
       <c r="K5" s="98"/>
     </row>
-    <row r="6" spans="1:11" s="9" customFormat="1" ht="12.75" thickBot="1">
+    <row r="6" spans="1:11" s="9" customFormat="1" ht="12.6" thickBot="1">
       <c r="A6" s="105"/>
       <c r="B6" s="43" t="s">
         <v>0</v>
@@ -2005,7 +2010,7 @@
       <c r="J6" s="30"/>
       <c r="K6" s="30"/>
     </row>
-    <row r="7" spans="1:11" ht="16.5" thickBot="1">
+    <row r="7" spans="1:11" ht="16.2" thickBot="1">
       <c r="A7" s="106"/>
       <c r="B7" s="69"/>
       <c r="C7" s="70">
@@ -2036,7 +2041,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16.5" thickBot="1">
+    <row r="8" spans="1:11" ht="16.2" thickBot="1">
       <c r="A8" s="106"/>
       <c r="B8" s="71"/>
       <c r="C8" s="72">
@@ -2080,7 +2085,7 @@
       <c r="J9" s="45"/>
       <c r="K9" s="45"/>
     </row>
-    <row r="10" spans="1:11" ht="16.5" thickBot="1">
+    <row r="10" spans="1:11" ht="16.2" thickBot="1">
       <c r="A10" s="61" t="s">
         <v>6</v>
       </c>
@@ -2115,7 +2120,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75">
+    <row r="11" spans="1:11" ht="15.6">
       <c r="A11" s="36" t="s">
         <v>2</v>
       </c>
@@ -2159,7 +2164,7 @@
         <v>4680</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75">
+    <row r="12" spans="1:11" ht="15.6">
       <c r="A12" s="37" t="s">
         <v>3</v>
       </c>
@@ -2203,7 +2208,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16.5" thickBot="1">
+    <row r="13" spans="1:11" ht="16.2" thickBot="1">
       <c r="A13" s="38" t="s">
         <v>4</v>
       </c>
@@ -2247,7 +2252,7 @@
         <v>7020.0000000000009</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75">
+    <row r="14" spans="1:11" ht="15.6">
       <c r="A14" s="39" t="s">
         <v>7</v>
       </c>
@@ -2291,7 +2296,7 @@
         <v>4680</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75">
+    <row r="15" spans="1:11" ht="15.6">
       <c r="A15" s="37" t="s">
         <v>9</v>
       </c>
@@ -2335,7 +2340,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75">
+    <row r="16" spans="1:11" ht="15.6">
       <c r="A16" s="40" t="s">
         <v>8</v>
       </c>
@@ -2379,7 +2384,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="16.5" thickBot="1">
+    <row r="17" spans="1:11" ht="16.2" thickBot="1">
       <c r="A17" s="41" t="s">
         <v>19</v>
       </c>
@@ -2671,7 +2676,7 @@
       <c r="J25" s="68"/>
       <c r="K25" s="68"/>
     </row>
-    <row r="26" spans="1:11" s="9" customFormat="1" ht="12.75" thickBot="1">
+    <row r="26" spans="1:11" s="9" customFormat="1" ht="12.6" thickBot="1">
       <c r="A26" s="42" t="s">
         <v>5</v>
       </c>
@@ -2704,7 +2709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="9" customFormat="1" ht="12.75" thickBot="1">
+    <row r="27" spans="1:11" s="9" customFormat="1" ht="12.6" thickBot="1">
       <c r="A27" s="42"/>
       <c r="B27" s="13"/>
       <c r="C27" s="48"/>
@@ -2717,7 +2722,7 @@
       <c r="J27" s="48"/>
       <c r="K27" s="48"/>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1">
+    <row r="28" spans="1:11" ht="14.4" thickBot="1">
       <c r="A28" s="42" t="s">
         <v>16</v>
       </c>
@@ -2750,7 +2755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75">
+    <row r="29" spans="1:11" ht="15.6">
       <c r="A29" s="49"/>
       <c r="B29" s="50"/>
       <c r="C29" s="51"/>
@@ -2763,7 +2768,7 @@
       <c r="J29" s="51"/>
       <c r="K29" s="52"/>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1">
+    <row r="30" spans="1:11" ht="14.4" thickBot="1">
       <c r="A30" s="33"/>
       <c r="B30" s="17"/>
       <c r="C30" s="18"/>
@@ -2776,7 +2781,7 @@
       <c r="J30" s="18"/>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75">
+    <row r="31" spans="1:11" ht="15.6">
       <c r="A31" s="20" t="s">
         <v>10</v>
       </c>
@@ -2791,7 +2796,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="16"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75">
+    <row r="32" spans="1:11" ht="15.6">
       <c r="A32" s="22" t="s">
         <v>20</v>
       </c>
@@ -2851,7 +2856,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="16"/>
     </row>
-    <row r="36" spans="1:11" ht="15" thickBot="1">
+    <row r="36" spans="1:11" ht="14.4" thickBot="1">
       <c r="A36" s="27" t="s">
         <v>14</v>
       </c>

</xml_diff>